<commit_message>
log log graphs of retweets and updated getting favorite scripts
</commit_message>
<xml_diff>
--- a/twitter_data/Retweet_FavAnalysis.xlsx
+++ b/twitter_data/Retweet_FavAnalysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,12 +260,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2019850624"/>
-        <c:axId val="-2030956944"/>
+        <c:axId val="2141215760"/>
+        <c:axId val="2141222512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2019850624"/>
+        <c:axId val="2141215760"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -321,13 +322,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2030956944"/>
+        <c:crossAx val="2141222512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2030956944"/>
+        <c:axId val="2141222512"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -383,7 +385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019850624"/>
+        <c:crossAx val="2141215760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -629,12 +631,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2021172784"/>
-        <c:axId val="-2020805392"/>
+        <c:axId val="-2101244096"/>
+        <c:axId val="-2101237888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2021172784"/>
+        <c:axId val="-2101244096"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -690,13 +693,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2020805392"/>
+        <c:crossAx val="-2101237888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2020805392"/>
+        <c:axId val="-2101237888"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -752,7 +756,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2021172784"/>
+        <c:crossAx val="-2101244096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1003,12 +1007,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2076519376"/>
-        <c:axId val="-2076490416"/>
+        <c:axId val="-2101212944"/>
+        <c:axId val="-2101206736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2076519376"/>
+        <c:axId val="-2101212944"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1064,13 +1069,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076490416"/>
+        <c:crossAx val="-2101206736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076490416"/>
+        <c:axId val="-2101206736"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1126,7 +1132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076519376"/>
+        <c:crossAx val="-2101212944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3203,8 +3209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:B38"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
script to parse followers and followings from db for placement into db, networking stuff for second dataset, updated 2nd table in db
</commit_message>
<xml_diff>
--- a/twitter_data/Retweet_FavAnalysis.xlsx
+++ b/twitter_data/Retweet_FavAnalysis.xlsx
@@ -23,12 +23,51 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>0_1</t>
+  </si>
+  <si>
+    <t>2_5</t>
+  </si>
+  <si>
+    <t>6_10</t>
+  </si>
+  <si>
+    <t>11_25</t>
+  </si>
+  <si>
+    <t>26_50</t>
+  </si>
+  <si>
+    <t>51_100</t>
+  </si>
+  <si>
+    <t>101_150</t>
+  </si>
+  <si>
+    <t>151_200</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,8 +93,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,44 +227,41 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$1:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>150.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>200.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>500.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="9"/>
+              <c:pt idx="0">
+                <c:v>1.0</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>5.0</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>10.0</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>25.0</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50.0</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>100.0</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>150.0</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>200.0</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>500.0</c:v>
+              </c:pt>
+            </c:numLit>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$9</c:f>
+              <c:f>Sheet1!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -260,11 +305,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141215760"/>
-        <c:axId val="2141222512"/>
+        <c:axId val="1792463808"/>
+        <c:axId val="1792376608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141215760"/>
+        <c:axId val="1792463808"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -322,12 +367,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141222512"/>
+        <c:crossAx val="1792376608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141222512"/>
+        <c:axId val="1792376608"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -385,7 +430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141215760"/>
+        <c:crossAx val="1792463808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -545,10 +590,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$15:$A$24</c:f>
+              <c:f>Sheet1!$A$14:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -584,10 +629,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$24</c:f>
+              <c:f>Sheet1!$B$14:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1236.0</c:v>
                 </c:pt>
@@ -631,11 +676,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2101244096"/>
-        <c:axId val="-2101237888"/>
+        <c:axId val="1792768576"/>
+        <c:axId val="1792774704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2101244096"/>
+        <c:axId val="1792768576"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -693,12 +738,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101237888"/>
+        <c:crossAx val="1792774704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2101237888"/>
+        <c:axId val="1792774704"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -756,7 +801,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101244096"/>
+        <c:crossAx val="1792768576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1007,11 +1052,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2101212944"/>
-        <c:axId val="-2101206736"/>
+        <c:axId val="1792799376"/>
+        <c:axId val="1792805520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2101212944"/>
+        <c:axId val="1792799376"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1069,12 +1114,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101206736"/>
+        <c:crossAx val="1792805520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2101206736"/>
+        <c:axId val="1792805520"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1132,7 +1177,737 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101212944"/>
+        <c:crossAx val="1792799376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Retweet Count</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4272.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1792831024"/>
+        <c:axId val="1792837152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1792831024"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1792837152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1792837152"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1792831024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Favorite Count</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$15:$J$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$15:$K$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3273.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>969.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>167.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1792862096"/>
+        <c:axId val="1792868320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1792862096"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1792868320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1792868320"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1792862096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1301,6 +2076,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2334,6 +3189,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2936,6 +4823,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3207,175 +5154,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
       <c r="B1">
+        <v>3945</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>5</v>
+      </c>
+      <c r="B2">
         <v>1380</v>
       </c>
+      <c r="I2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>4272</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>341</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>341</v>
+      <c r="K3" s="2">
+        <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>134</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>134</v>
+      <c r="K4" s="2">
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>44</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
         <v>25</v>
       </c>
-      <c r="B4">
-        <v>44</v>
+      <c r="K5" s="2">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>100</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1">
         <v>50</v>
       </c>
-      <c r="B5">
-        <v>22</v>
+      <c r="K6" s="2">
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>150</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1">
         <v>100</v>
       </c>
-      <c r="B6">
-        <v>9</v>
+      <c r="K7" s="2">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>200</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="1">
         <v>150</v>
       </c>
-      <c r="B7">
-        <v>6</v>
+      <c r="K8" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>200</v>
-      </c>
-      <c r="B8">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>500</v>
+      </c>
+      <c r="B9">
         <v>3</v>
       </c>
+      <c r="I9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2000</v>
+      </c>
+      <c r="K9" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>500</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1000</v>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>2000</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>1</v>
       </c>
-      <c r="B15">
+      <c r="B14" s="3">
         <v>1236</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="B15" s="3">
         <v>267</v>
       </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2">
+        <v>3273</v>
+      </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
         <v>10</v>
       </c>
-      <c r="B17">
+      <c r="B16" s="3">
         <v>100</v>
       </c>
+      <c r="J16" s="1">
+        <v>5</v>
+      </c>
+      <c r="K16" s="2">
+        <v>969</v>
+      </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <v>25</v>
       </c>
-      <c r="B18">
+      <c r="B17" s="3">
         <v>30</v>
       </c>
+      <c r="J17" s="1">
+        <v>10</v>
+      </c>
+      <c r="K17" s="2">
+        <v>167</v>
+      </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>50</v>
       </c>
-      <c r="B19">
+      <c r="B18" s="3">
         <v>19</v>
       </c>
+      <c r="J18" s="1">
+        <v>25</v>
+      </c>
+      <c r="K18" s="2">
+        <v>70</v>
+      </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <v>100</v>
       </c>
-      <c r="B20">
+      <c r="B19" s="3">
         <v>6</v>
       </c>
+      <c r="J19" s="1">
+        <v>50</v>
+      </c>
+      <c r="K19" s="2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>150</v>
       </c>
-      <c r="B21">
+      <c r="B20" s="3">
         <v>5</v>
       </c>
+      <c r="J20" s="1">
+        <v>100</v>
+      </c>
+      <c r="K20" s="2">
+        <v>13</v>
+      </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>200</v>
       </c>
-      <c r="B22">
+      <c r="B21" s="3">
         <v>4</v>
       </c>
+      <c r="J21" s="1">
+        <v>150</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>500</v>
       </c>
-      <c r="B23">
+      <c r="B22" s="3">
         <v>2</v>
       </c>
+      <c r="J22" s="1">
+        <v>200</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>1000</v>
       </c>
-      <c r="B24">
+      <c r="B23" s="3">
         <v>2</v>
       </c>
+      <c r="J23" s="1">
+        <v>500</v>
+      </c>
+      <c r="K23" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="J24" s="1">
+        <v>2000</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J25" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -3383,7 +5486,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>5</v>
       </c>
@@ -3391,7 +5494,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>10</v>
       </c>
@@ -3399,7 +5502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>25</v>
       </c>
@@ -3407,7 +5510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>50</v>
       </c>
@@ -3415,15 +5518,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>100</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
+      <c r="J34" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>150</v>
       </c>
@@ -3431,7 +5537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>200</v>
       </c>
@@ -3439,7 +5545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>500</v>
       </c>
@@ -3447,7 +5553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1000</v>
       </c>
@@ -3455,7 +5561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2000</v>
       </c>
@@ -3465,6 +5571,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>